<commit_message>
Alterados promenores da Especificações de Use Cases
</commit_message>
<xml_diff>
--- a/Fase2/UML/Especificação de Use Cases/Editar lista de Materiais.xlsx
+++ b/Fase2/UML/Especificação de Use Cases/Editar lista de Materiais.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Google Drive\Universidade\3º + 2º Ano_\2º Semestre\LI4\Especificação de Use Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\OneDrive\Documents\GitHub\li4-17-18\Fase2\UML\Especificação de Use Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5102E0B3-8FAA-4D1C-93E6-A2CF29C2A735}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EDA685-7EE8-4830-B857-C9219D9C93C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{989698FE-73B3-4F92-89E4-B8E9AE1BA80B}"/>
   </bookViews>
@@ -112,9 +112,6 @@
     <t>Lista de Materiais editada</t>
   </si>
   <si>
-    <t>Pede para editar lista de Materiais</t>
-  </si>
-  <si>
     <t>Apresenta lista de Materiais</t>
   </si>
   <si>
@@ -125,6 +122,9 @@
   </si>
   <si>
     <t>Informa que a lista foi editada com sucesso</t>
+  </si>
+  <si>
+    <t>Indica que pretende editar lista de Materiais</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +603,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -614,7 +614,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -623,7 +623,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -634,7 +634,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -644,7 +644,7 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>